<commit_message>
Project 4 updated gantt
</commit_message>
<xml_diff>
--- a/documentation/ProjectGanttChart.xlsx
+++ b/documentation/ProjectGanttChart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anton\Desktop\448\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5AD9653-53ED-44D5-8E4E-0E6A7936DE1A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{694824D7-2820-468C-8444-7409B4AE39C0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Gantt Chart w % Complete" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="84">
   <si>
     <t>GANTT CHART TEMPLATE</t>
   </si>
@@ -269,9 +269,6 @@
     <t>Report Feature</t>
   </si>
   <si>
-    <t>TBA</t>
-  </si>
-  <si>
     <t>Adding tags to answers</t>
   </si>
   <si>
@@ -282,6 +279,9 @@
   </si>
   <si>
     <t>KRAAG Courses ++</t>
+  </si>
+  <si>
+    <t>Test Suite</t>
   </si>
 </sst>
 </file>
@@ -694,7 +694,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="101">
+  <cellXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -857,6 +857,8 @@
     <xf numFmtId="0" fontId="9" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2841,80 +2843,80 @@
       <c r="AJ5" s="2"/>
     </row>
     <row r="6" spans="1:36" ht="14.35">
-      <c r="A6" s="86"/>
-      <c r="B6" s="86" t="s">
+      <c r="A6" s="88"/>
+      <c r="B6" s="88" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="86" t="s">
+      <c r="C6" s="88" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="86" t="s">
+      <c r="D6" s="88" t="s">
         <v>42</v>
       </c>
-      <c r="E6" s="86" t="s">
+      <c r="E6" s="88" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="86" t="s">
+      <c r="F6" s="88" t="s">
         <v>41</v>
       </c>
-      <c r="G6" s="86" t="s">
+      <c r="G6" s="88" t="s">
         <v>43</v>
       </c>
-      <c r="H6" s="86" t="s">
+      <c r="H6" s="88" t="s">
         <v>44</v>
       </c>
-      <c r="I6" s="86" t="s">
+      <c r="I6" s="88" t="s">
         <v>5</v>
       </c>
-      <c r="J6" s="86" t="s">
+      <c r="J6" s="88" t="s">
         <v>6</v>
       </c>
-      <c r="K6" s="89"/>
-      <c r="L6" s="87"/>
-      <c r="M6" s="87"/>
-      <c r="N6" s="87"/>
-      <c r="O6" s="87"/>
-      <c r="P6" s="89" t="s">
+      <c r="K6" s="91"/>
+      <c r="L6" s="89"/>
+      <c r="M6" s="89"/>
+      <c r="N6" s="89"/>
+      <c r="O6" s="89"/>
+      <c r="P6" s="91" t="s">
         <v>7</v>
       </c>
-      <c r="Q6" s="87"/>
-      <c r="R6" s="87"/>
-      <c r="S6" s="87"/>
-      <c r="T6" s="87"/>
-      <c r="U6" s="88" t="s">
+      <c r="Q6" s="89"/>
+      <c r="R6" s="89"/>
+      <c r="S6" s="89"/>
+      <c r="T6" s="89"/>
+      <c r="U6" s="90" t="s">
         <v>8</v>
       </c>
-      <c r="V6" s="87"/>
-      <c r="W6" s="87"/>
-      <c r="X6" s="87"/>
-      <c r="Y6" s="87"/>
-      <c r="Z6" s="89" t="s">
+      <c r="V6" s="89"/>
+      <c r="W6" s="89"/>
+      <c r="X6" s="89"/>
+      <c r="Y6" s="89"/>
+      <c r="Z6" s="91" t="s">
         <v>9</v>
       </c>
-      <c r="AA6" s="87"/>
-      <c r="AB6" s="87"/>
-      <c r="AC6" s="87"/>
-      <c r="AD6" s="87"/>
-      <c r="AE6" s="88" t="s">
+      <c r="AA6" s="89"/>
+      <c r="AB6" s="89"/>
+      <c r="AC6" s="89"/>
+      <c r="AD6" s="89"/>
+      <c r="AE6" s="90" t="s">
         <v>10</v>
       </c>
-      <c r="AF6" s="87"/>
-      <c r="AG6" s="87"/>
-      <c r="AH6" s="87"/>
-      <c r="AI6" s="87"/>
+      <c r="AF6" s="89"/>
+      <c r="AG6" s="89"/>
+      <c r="AH6" s="89"/>
+      <c r="AI6" s="89"/>
       <c r="AJ6" s="43"/>
     </row>
     <row r="7" spans="1:36" ht="14.35">
-      <c r="A7" s="87"/>
-      <c r="B7" s="87"/>
-      <c r="C7" s="87"/>
-      <c r="D7" s="87"/>
-      <c r="E7" s="87"/>
-      <c r="F7" s="87"/>
-      <c r="G7" s="87"/>
-      <c r="H7" s="87"/>
-      <c r="I7" s="87"/>
-      <c r="J7" s="87"/>
+      <c r="A7" s="89"/>
+      <c r="B7" s="89"/>
+      <c r="C7" s="89"/>
+      <c r="D7" s="89"/>
+      <c r="E7" s="89"/>
+      <c r="F7" s="89"/>
+      <c r="G7" s="89"/>
+      <c r="H7" s="89"/>
+      <c r="I7" s="89"/>
+      <c r="J7" s="89"/>
       <c r="K7" s="43"/>
       <c r="L7" s="43"/>
       <c r="M7" s="43"/>
@@ -3887,16 +3889,16 @@
       <c r="AH2" s="2"/>
     </row>
     <row r="3" spans="1:34" ht="30" customHeight="1">
-      <c r="A3" s="90" t="s">
+      <c r="A3" s="92" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="91"/>
-      <c r="C3" s="91"/>
-      <c r="D3" s="91"/>
-      <c r="E3" s="91"/>
-      <c r="F3" s="91"/>
-      <c r="G3" s="91"/>
-      <c r="H3" s="91"/>
+      <c r="B3" s="93"/>
+      <c r="C3" s="93"/>
+      <c r="D3" s="93"/>
+      <c r="E3" s="93"/>
+      <c r="F3" s="93"/>
+      <c r="G3" s="93"/>
+      <c r="H3" s="93"/>
       <c r="I3" s="5"/>
       <c r="J3" s="6"/>
       <c r="K3" s="6"/>
@@ -3998,72 +4000,72 @@
       <c r="AH5" s="2"/>
     </row>
     <row r="6" spans="1:34" ht="14.35">
-      <c r="A6" s="86"/>
-      <c r="B6" s="86" t="s">
+      <c r="A6" s="88"/>
+      <c r="B6" s="88" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="86" t="s">
+      <c r="C6" s="88" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="86" t="s">
+      <c r="D6" s="88" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="86" t="s">
+      <c r="E6" s="88" t="s">
         <v>40</v>
       </c>
-      <c r="F6" s="86" t="s">
+      <c r="F6" s="88" t="s">
         <v>41</v>
       </c>
-      <c r="G6" s="86" t="s">
+      <c r="G6" s="88" t="s">
         <v>5</v>
       </c>
-      <c r="H6" s="86" t="s">
+      <c r="H6" s="88" t="s">
         <v>6</v>
       </c>
-      <c r="I6" s="89"/>
-      <c r="J6" s="87"/>
-      <c r="K6" s="87"/>
-      <c r="L6" s="87"/>
-      <c r="M6" s="87"/>
-      <c r="N6" s="89" t="s">
+      <c r="I6" s="91"/>
+      <c r="J6" s="89"/>
+      <c r="K6" s="89"/>
+      <c r="L6" s="89"/>
+      <c r="M6" s="89"/>
+      <c r="N6" s="91" t="s">
         <v>7</v>
       </c>
-      <c r="O6" s="87"/>
-      <c r="P6" s="87"/>
-      <c r="Q6" s="87"/>
-      <c r="R6" s="87"/>
-      <c r="S6" s="88" t="s">
+      <c r="O6" s="89"/>
+      <c r="P6" s="89"/>
+      <c r="Q6" s="89"/>
+      <c r="R6" s="89"/>
+      <c r="S6" s="90" t="s">
         <v>8</v>
       </c>
-      <c r="T6" s="87"/>
-      <c r="U6" s="87"/>
-      <c r="V6" s="87"/>
-      <c r="W6" s="87"/>
-      <c r="X6" s="89" t="s">
+      <c r="T6" s="89"/>
+      <c r="U6" s="89"/>
+      <c r="V6" s="89"/>
+      <c r="W6" s="89"/>
+      <c r="X6" s="91" t="s">
         <v>9</v>
       </c>
-      <c r="Y6" s="87"/>
-      <c r="Z6" s="87"/>
-      <c r="AA6" s="87"/>
-      <c r="AB6" s="87"/>
-      <c r="AC6" s="88" t="s">
+      <c r="Y6" s="89"/>
+      <c r="Z6" s="89"/>
+      <c r="AA6" s="89"/>
+      <c r="AB6" s="89"/>
+      <c r="AC6" s="90" t="s">
         <v>10</v>
       </c>
-      <c r="AD6" s="87"/>
-      <c r="AE6" s="87"/>
-      <c r="AF6" s="87"/>
-      <c r="AG6" s="87"/>
+      <c r="AD6" s="89"/>
+      <c r="AE6" s="89"/>
+      <c r="AF6" s="89"/>
+      <c r="AG6" s="89"/>
       <c r="AH6" s="43"/>
     </row>
     <row r="7" spans="1:34" ht="14.35">
-      <c r="A7" s="87"/>
-      <c r="B7" s="87"/>
-      <c r="C7" s="87"/>
-      <c r="D7" s="87"/>
-      <c r="E7" s="87"/>
-      <c r="F7" s="87"/>
-      <c r="G7" s="87"/>
-      <c r="H7" s="87"/>
+      <c r="A7" s="89"/>
+      <c r="B7" s="89"/>
+      <c r="C7" s="89"/>
+      <c r="D7" s="89"/>
+      <c r="E7" s="89"/>
+      <c r="F7" s="89"/>
+      <c r="G7" s="89"/>
+      <c r="H7" s="89"/>
       <c r="I7" s="43"/>
       <c r="J7" s="43"/>
       <c r="K7" s="43"/>
@@ -4780,10 +4782,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:BO990"/>
+  <dimension ref="A1:BO991"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="M25" sqref="M25"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.46875" defaultRowHeight="15.75" customHeight="1"/>
@@ -4936,15 +4938,15 @@
       <c r="BO2" s="2"/>
     </row>
     <row r="3" spans="1:67" ht="30" customHeight="1">
-      <c r="A3" s="94" t="s">
-        <v>83</v>
-      </c>
-      <c r="B3" s="91"/>
-      <c r="C3" s="91"/>
-      <c r="D3" s="91"/>
-      <c r="E3" s="91"/>
-      <c r="F3" s="91"/>
-      <c r="G3" s="91"/>
+      <c r="A3" s="96" t="s">
+        <v>82</v>
+      </c>
+      <c r="B3" s="93"/>
+      <c r="C3" s="93"/>
+      <c r="D3" s="93"/>
+      <c r="E3" s="93"/>
+      <c r="F3" s="93"/>
+      <c r="G3" s="93"/>
       <c r="H3" s="5"/>
       <c r="I3" s="6"/>
       <c r="J3" s="6"/>
@@ -5145,118 +5147,118 @@
       <c r="BO5" s="2"/>
     </row>
     <row r="6" spans="1:67" ht="14.35">
-      <c r="A6" s="86"/>
-      <c r="B6" s="86" t="s">
+      <c r="A6" s="88"/>
+      <c r="B6" s="88" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="86" t="s">
+      <c r="C6" s="88" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="86" t="s">
+      <c r="D6" s="88" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="86" t="s">
+      <c r="E6" s="88" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="86" t="s">
+      <c r="F6" s="88" t="s">
         <v>5</v>
       </c>
-      <c r="G6" s="95" t="s">
+      <c r="G6" s="97" t="s">
         <v>6</v>
       </c>
-      <c r="H6" s="97" t="s">
+      <c r="H6" s="99" t="s">
         <v>7</v>
       </c>
-      <c r="I6" s="93"/>
-      <c r="J6" s="93"/>
-      <c r="K6" s="93"/>
-      <c r="L6" s="93"/>
-      <c r="M6" s="92" t="s">
+      <c r="I6" s="95"/>
+      <c r="J6" s="95"/>
+      <c r="K6" s="95"/>
+      <c r="L6" s="95"/>
+      <c r="M6" s="94" t="s">
         <v>8</v>
       </c>
-      <c r="N6" s="93"/>
-      <c r="O6" s="93"/>
-      <c r="P6" s="93"/>
-      <c r="Q6" s="93"/>
-      <c r="R6" s="97" t="s">
+      <c r="N6" s="95"/>
+      <c r="O6" s="95"/>
+      <c r="P6" s="95"/>
+      <c r="Q6" s="95"/>
+      <c r="R6" s="99" t="s">
         <v>9</v>
       </c>
-      <c r="S6" s="93"/>
-      <c r="T6" s="93"/>
-      <c r="U6" s="93"/>
-      <c r="V6" s="93"/>
-      <c r="W6" s="92" t="s">
+      <c r="S6" s="95"/>
+      <c r="T6" s="95"/>
+      <c r="U6" s="95"/>
+      <c r="V6" s="95"/>
+      <c r="W6" s="94" t="s">
         <v>10</v>
       </c>
-      <c r="X6" s="93"/>
-      <c r="Y6" s="93"/>
-      <c r="Z6" s="93"/>
-      <c r="AA6" s="93"/>
-      <c r="AB6" s="97" t="s">
+      <c r="X6" s="95"/>
+      <c r="Y6" s="95"/>
+      <c r="Z6" s="95"/>
+      <c r="AA6" s="95"/>
+      <c r="AB6" s="99" t="s">
         <v>11</v>
       </c>
-      <c r="AC6" s="93"/>
-      <c r="AD6" s="93"/>
-      <c r="AE6" s="93"/>
-      <c r="AF6" s="93"/>
-      <c r="AG6" s="92" t="s">
+      <c r="AC6" s="95"/>
+      <c r="AD6" s="95"/>
+      <c r="AE6" s="95"/>
+      <c r="AF6" s="95"/>
+      <c r="AG6" s="94" t="s">
         <v>12</v>
       </c>
-      <c r="AH6" s="93"/>
-      <c r="AI6" s="93"/>
-      <c r="AJ6" s="93"/>
-      <c r="AK6" s="93"/>
-      <c r="AL6" s="97" t="s">
+      <c r="AH6" s="95"/>
+      <c r="AI6" s="95"/>
+      <c r="AJ6" s="95"/>
+      <c r="AK6" s="95"/>
+      <c r="AL6" s="99" t="s">
         <v>13</v>
       </c>
-      <c r="AM6" s="93"/>
-      <c r="AN6" s="93"/>
-      <c r="AO6" s="93"/>
-      <c r="AP6" s="93"/>
-      <c r="AQ6" s="92" t="s">
+      <c r="AM6" s="95"/>
+      <c r="AN6" s="95"/>
+      <c r="AO6" s="95"/>
+      <c r="AP6" s="95"/>
+      <c r="AQ6" s="94" t="s">
         <v>14</v>
       </c>
-      <c r="AR6" s="93"/>
-      <c r="AS6" s="93"/>
-      <c r="AT6" s="93"/>
-      <c r="AU6" s="93"/>
-      <c r="AV6" s="97" t="s">
+      <c r="AR6" s="95"/>
+      <c r="AS6" s="95"/>
+      <c r="AT6" s="95"/>
+      <c r="AU6" s="95"/>
+      <c r="AV6" s="99" t="s">
         <v>15</v>
       </c>
-      <c r="AW6" s="93"/>
-      <c r="AX6" s="93"/>
-      <c r="AY6" s="93"/>
-      <c r="AZ6" s="93"/>
-      <c r="BA6" s="92" t="s">
+      <c r="AW6" s="95"/>
+      <c r="AX6" s="95"/>
+      <c r="AY6" s="95"/>
+      <c r="AZ6" s="95"/>
+      <c r="BA6" s="94" t="s">
         <v>16</v>
       </c>
-      <c r="BB6" s="93"/>
-      <c r="BC6" s="93"/>
-      <c r="BD6" s="93"/>
-      <c r="BE6" s="93"/>
-      <c r="BF6" s="97" t="s">
+      <c r="BB6" s="95"/>
+      <c r="BC6" s="95"/>
+      <c r="BD6" s="95"/>
+      <c r="BE6" s="95"/>
+      <c r="BF6" s="99" t="s">
         <v>17</v>
       </c>
-      <c r="BG6" s="93"/>
-      <c r="BH6" s="93"/>
-      <c r="BI6" s="93"/>
-      <c r="BJ6" s="93"/>
-      <c r="BK6" s="92" t="s">
+      <c r="BG6" s="95"/>
+      <c r="BH6" s="95"/>
+      <c r="BI6" s="95"/>
+      <c r="BJ6" s="95"/>
+      <c r="BK6" s="94" t="s">
         <v>18</v>
       </c>
-      <c r="BL6" s="93"/>
-      <c r="BM6" s="93"/>
-      <c r="BN6" s="93"/>
-      <c r="BO6" s="93"/>
+      <c r="BL6" s="95"/>
+      <c r="BM6" s="95"/>
+      <c r="BN6" s="95"/>
+      <c r="BO6" s="95"/>
     </row>
     <row r="7" spans="1:67" ht="14.35">
-      <c r="A7" s="87"/>
-      <c r="B7" s="87"/>
-      <c r="C7" s="87"/>
-      <c r="D7" s="87"/>
-      <c r="E7" s="87"/>
-      <c r="F7" s="87"/>
-      <c r="G7" s="96"/>
+      <c r="A7" s="89"/>
+      <c r="B7" s="89"/>
+      <c r="C7" s="89"/>
+      <c r="D7" s="89"/>
+      <c r="E7" s="89"/>
+      <c r="F7" s="89"/>
+      <c r="G7" s="98"/>
       <c r="H7" s="10" t="s">
         <v>19</v>
       </c>
@@ -5443,11 +5445,11 @@
         <v>69</v>
       </c>
       <c r="B8" s="15"/>
-      <c r="C8" s="100"/>
-      <c r="D8" s="99"/>
-      <c r="E8" s="99"/>
-      <c r="F8" s="99"/>
-      <c r="G8" s="99"/>
+      <c r="C8" s="102"/>
+      <c r="D8" s="101"/>
+      <c r="E8" s="101"/>
+      <c r="F8" s="101"/>
+      <c r="G8" s="101"/>
       <c r="H8" s="16"/>
       <c r="I8" s="17"/>
       <c r="J8" s="18"/>
@@ -6000,11 +6002,11 @@
         <v>70</v>
       </c>
       <c r="B15" s="30"/>
-      <c r="C15" s="98"/>
-      <c r="D15" s="99"/>
-      <c r="E15" s="99"/>
-      <c r="F15" s="99"/>
-      <c r="G15" s="99"/>
+      <c r="C15" s="100"/>
+      <c r="D15" s="101"/>
+      <c r="E15" s="101"/>
+      <c r="F15" s="101"/>
+      <c r="G15" s="101"/>
       <c r="H15" s="31"/>
       <c r="I15" s="32"/>
       <c r="J15" s="33"/>
@@ -6476,11 +6478,11 @@
         <v>77</v>
       </c>
       <c r="B21" s="30"/>
-      <c r="C21" s="98"/>
-      <c r="D21" s="99"/>
-      <c r="E21" s="99"/>
-      <c r="F21" s="99"/>
-      <c r="G21" s="99"/>
+      <c r="C21" s="100"/>
+      <c r="D21" s="101"/>
+      <c r="E21" s="101"/>
+      <c r="F21" s="101"/>
+      <c r="G21" s="101"/>
       <c r="H21" s="31"/>
       <c r="I21" s="32"/>
       <c r="J21" s="33"/>
@@ -6547,20 +6549,20 @@
         <v>78</v>
       </c>
       <c r="C22" s="34">
-        <v>43780</v>
+        <v>43785</v>
       </c>
       <c r="D22" s="34">
         <v>43799</v>
       </c>
       <c r="E22" s="21">
         <f>NETWORKDAYS(C22,D22)</f>
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F22" s="19" t="s">
-        <v>79</v>
+        <v>64</v>
       </c>
       <c r="G22" s="36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H22" s="23"/>
       <c r="I22" s="24"/>
@@ -6577,11 +6579,11 @@
       <c r="T22" s="25"/>
       <c r="U22" s="25"/>
       <c r="V22" s="25"/>
-      <c r="W22" s="26"/>
-      <c r="X22" s="26"/>
-      <c r="Y22" s="26"/>
-      <c r="Z22" s="26"/>
-      <c r="AA22" s="26"/>
+      <c r="W22" s="74"/>
+      <c r="X22" s="73"/>
+      <c r="Y22" s="73"/>
+      <c r="Z22" s="73"/>
+      <c r="AA22" s="73"/>
       <c r="AB22" s="27"/>
       <c r="AC22" s="27"/>
       <c r="AD22" s="27"/>
@@ -6625,23 +6627,23 @@
     </row>
     <row r="23" spans="1:67" ht="14.35">
       <c r="B23" s="19" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C23" s="34">
-        <v>43781</v>
+        <v>43785</v>
       </c>
       <c r="D23" s="34">
         <v>43799</v>
       </c>
       <c r="E23" s="21">
-        <f t="shared" ref="E23:E25" si="2">NETWORKDAYS(C23,D23)</f>
-        <v>14</v>
+        <f t="shared" ref="E23:E26" si="2">NETWORKDAYS(C23,D23)</f>
+        <v>10</v>
       </c>
       <c r="F23" s="19" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="G23" s="36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H23" s="23"/>
       <c r="I23" s="24"/>
@@ -6658,11 +6660,11 @@
       <c r="T23" s="25"/>
       <c r="U23" s="25"/>
       <c r="V23" s="25"/>
-      <c r="W23" s="26"/>
-      <c r="X23" s="26"/>
-      <c r="Y23" s="26"/>
-      <c r="Z23" s="26"/>
-      <c r="AA23" s="26"/>
+      <c r="W23" s="74"/>
+      <c r="X23" s="73"/>
+      <c r="Y23" s="73"/>
+      <c r="Z23" s="73"/>
+      <c r="AA23" s="73"/>
       <c r="AB23" s="27"/>
       <c r="AC23" s="27"/>
       <c r="AD23" s="27"/>
@@ -6706,23 +6708,23 @@
     </row>
     <row r="24" spans="1:67" ht="14.35">
       <c r="B24" s="19" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C24" s="34">
-        <v>43783</v>
+        <v>43785</v>
       </c>
       <c r="D24" s="34">
         <v>43800</v>
       </c>
       <c r="E24" s="21">
         <f t="shared" si="2"/>
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F24" s="19" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="G24" s="36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H24" s="23"/>
       <c r="I24" s="24"/>
@@ -6739,11 +6741,11 @@
       <c r="T24" s="25"/>
       <c r="U24" s="25"/>
       <c r="V24" s="25"/>
-      <c r="W24" s="26"/>
-      <c r="X24" s="26"/>
-      <c r="Y24" s="26"/>
-      <c r="Z24" s="26"/>
-      <c r="AA24" s="26"/>
+      <c r="W24" s="74"/>
+      <c r="X24" s="73"/>
+      <c r="Y24" s="73"/>
+      <c r="Z24" s="73"/>
+      <c r="AA24" s="73"/>
       <c r="AB24" s="27"/>
       <c r="AC24" s="27"/>
       <c r="AD24" s="27"/>
@@ -6785,25 +6787,25 @@
       <c r="BN24" s="26"/>
       <c r="BO24" s="28"/>
     </row>
-    <row r="25" spans="1:67" ht="14.35">
+    <row r="25" spans="1:67" s="86" customFormat="1" ht="14.35">
       <c r="B25" s="19" t="s">
-        <v>82</v>
+        <v>59</v>
       </c>
       <c r="C25" s="34">
-        <v>43782</v>
+        <v>43785</v>
       </c>
       <c r="D25" s="34">
         <v>43800</v>
       </c>
       <c r="E25" s="21">
         <f t="shared" si="2"/>
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F25" s="19" t="s">
-        <v>79</v>
+        <v>60</v>
       </c>
       <c r="G25" s="36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H25" s="23"/>
       <c r="I25" s="24"/>
@@ -6820,11 +6822,11 @@
       <c r="T25" s="25"/>
       <c r="U25" s="25"/>
       <c r="V25" s="25"/>
-      <c r="W25" s="26"/>
-      <c r="X25" s="26"/>
-      <c r="Y25" s="26"/>
-      <c r="Z25" s="26"/>
-      <c r="AA25" s="26"/>
+      <c r="W25" s="74"/>
+      <c r="X25" s="73"/>
+      <c r="Y25" s="73"/>
+      <c r="Z25" s="73"/>
+      <c r="AA25" s="73"/>
       <c r="AB25" s="27"/>
       <c r="AC25" s="27"/>
       <c r="AD25" s="27"/>
@@ -6866,177 +6868,177 @@
       <c r="BN25" s="26"/>
       <c r="BO25" s="28"/>
     </row>
-    <row r="26" spans="1:67" s="84" customFormat="1" ht="15.7">
-      <c r="A26" s="14" t="s">
+    <row r="26" spans="1:67" ht="14.35">
+      <c r="B26" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="C26" s="34">
+        <v>43785</v>
+      </c>
+      <c r="D26" s="34">
+        <v>43800</v>
+      </c>
+      <c r="E26" s="21">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="F26" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="G26" s="36">
+        <v>1</v>
+      </c>
+      <c r="H26" s="23"/>
+      <c r="I26" s="24"/>
+      <c r="J26" s="25"/>
+      <c r="K26" s="25"/>
+      <c r="L26" s="25"/>
+      <c r="M26" s="26"/>
+      <c r="N26" s="26"/>
+      <c r="O26" s="26"/>
+      <c r="P26" s="26"/>
+      <c r="Q26" s="26"/>
+      <c r="R26" s="25"/>
+      <c r="S26" s="25"/>
+      <c r="T26" s="25"/>
+      <c r="U26" s="25"/>
+      <c r="V26" s="25"/>
+      <c r="W26" s="74"/>
+      <c r="X26" s="73"/>
+      <c r="Y26" s="73"/>
+      <c r="Z26" s="73"/>
+      <c r="AA26" s="73"/>
+      <c r="AB26" s="27"/>
+      <c r="AC26" s="27"/>
+      <c r="AD26" s="27"/>
+      <c r="AE26" s="27"/>
+      <c r="AF26" s="27"/>
+      <c r="AG26" s="26"/>
+      <c r="AH26" s="26"/>
+      <c r="AI26" s="26"/>
+      <c r="AJ26" s="26"/>
+      <c r="AK26" s="26"/>
+      <c r="AL26" s="27"/>
+      <c r="AM26" s="27"/>
+      <c r="AN26" s="27"/>
+      <c r="AO26" s="27"/>
+      <c r="AP26" s="27"/>
+      <c r="AQ26" s="26"/>
+      <c r="AR26" s="26"/>
+      <c r="AS26" s="26"/>
+      <c r="AT26" s="26"/>
+      <c r="AU26" s="26"/>
+      <c r="AV26" s="25"/>
+      <c r="AW26" s="25"/>
+      <c r="AX26" s="25"/>
+      <c r="AY26" s="25"/>
+      <c r="AZ26" s="25"/>
+      <c r="BA26" s="26"/>
+      <c r="BB26" s="26"/>
+      <c r="BC26" s="26"/>
+      <c r="BD26" s="26"/>
+      <c r="BE26" s="26"/>
+      <c r="BF26" s="27"/>
+      <c r="BG26" s="27"/>
+      <c r="BH26" s="27"/>
+      <c r="BI26" s="27"/>
+      <c r="BJ26" s="27"/>
+      <c r="BK26" s="26"/>
+      <c r="BL26" s="26"/>
+      <c r="BM26" s="26"/>
+      <c r="BN26" s="26"/>
+      <c r="BO26" s="28"/>
+    </row>
+    <row r="27" spans="1:67" s="84" customFormat="1" ht="15.7">
+      <c r="A27" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="B26" s="85"/>
-      <c r="C26" s="98"/>
-      <c r="D26" s="99"/>
-      <c r="E26" s="99"/>
-      <c r="F26" s="99"/>
-      <c r="G26" s="99"/>
-      <c r="H26" s="31"/>
-      <c r="I26" s="32"/>
-      <c r="J26" s="33"/>
-      <c r="K26" s="33"/>
-      <c r="L26" s="72"/>
-      <c r="M26" s="72"/>
-      <c r="N26" s="72"/>
-      <c r="O26" s="72"/>
-      <c r="P26" s="72"/>
-      <c r="Q26" s="72"/>
-      <c r="R26" s="72"/>
-      <c r="S26" s="31"/>
-      <c r="T26" s="31"/>
-      <c r="U26" s="31"/>
-      <c r="V26" s="31"/>
-      <c r="W26" s="31"/>
-      <c r="X26" s="31"/>
-      <c r="Y26" s="31"/>
-      <c r="Z26" s="31"/>
-      <c r="AA26" s="31"/>
-      <c r="AB26" s="31"/>
-      <c r="AC26" s="31"/>
-      <c r="AD26" s="31"/>
-      <c r="AE26" s="31"/>
-      <c r="AF26" s="31"/>
-      <c r="AG26" s="31"/>
-      <c r="AH26" s="31"/>
-      <c r="AI26" s="31"/>
-      <c r="AJ26" s="31"/>
-      <c r="AK26" s="31"/>
-      <c r="AL26" s="31"/>
-      <c r="AM26" s="31"/>
-      <c r="AN26" s="31"/>
-      <c r="AO26" s="31"/>
-      <c r="AP26" s="31"/>
-      <c r="AQ26" s="31"/>
-      <c r="AR26" s="31"/>
-      <c r="AS26" s="31"/>
-      <c r="AT26" s="31"/>
-      <c r="AU26" s="31"/>
-      <c r="AV26" s="31"/>
-      <c r="AW26" s="31"/>
-      <c r="AX26" s="31"/>
-      <c r="AY26" s="31"/>
-      <c r="AZ26" s="31"/>
-      <c r="BA26" s="31"/>
-      <c r="BB26" s="31"/>
-      <c r="BC26" s="31"/>
-      <c r="BD26" s="31"/>
-      <c r="BE26" s="31"/>
-      <c r="BF26" s="31"/>
-      <c r="BG26" s="31"/>
-      <c r="BH26" s="31"/>
-      <c r="BI26" s="31"/>
-      <c r="BJ26" s="31"/>
-      <c r="BK26" s="31"/>
-      <c r="BL26" s="31"/>
-      <c r="BM26" s="31"/>
-      <c r="BN26" s="31"/>
-      <c r="BO26" s="31"/>
-    </row>
-    <row r="27" spans="1:67" s="84" customFormat="1" ht="14.35">
-      <c r="B27" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="C27" s="34">
-        <v>43780</v>
-      </c>
-      <c r="D27" s="34">
-        <v>43800</v>
-      </c>
-      <c r="E27" s="21">
-        <f>NETWORKDAYS(C27,D27)</f>
-        <v>15</v>
-      </c>
-      <c r="F27" s="19" t="s">
-        <v>58</v>
-      </c>
-      <c r="G27" s="35">
-        <v>0</v>
-      </c>
-      <c r="H27" s="23"/>
-      <c r="I27" s="24"/>
-      <c r="J27" s="25"/>
-      <c r="K27" s="25"/>
-      <c r="L27" s="25"/>
-      <c r="M27" s="26"/>
-      <c r="N27" s="26"/>
-      <c r="O27" s="26"/>
-      <c r="P27" s="26"/>
-      <c r="Q27" s="26"/>
-      <c r="R27" s="25"/>
-      <c r="S27" s="25"/>
-      <c r="T27" s="25"/>
-      <c r="U27" s="25"/>
-      <c r="V27" s="25"/>
-      <c r="W27" s="26"/>
-      <c r="X27" s="26"/>
-      <c r="Y27" s="26"/>
-      <c r="Z27" s="26"/>
-      <c r="AA27" s="26"/>
-      <c r="AB27" s="27"/>
-      <c r="AC27" s="27"/>
-      <c r="AD27" s="27"/>
-      <c r="AE27" s="27"/>
-      <c r="AF27" s="27"/>
-      <c r="AG27" s="26"/>
-      <c r="AH27" s="26"/>
-      <c r="AI27" s="26"/>
-      <c r="AJ27" s="26"/>
-      <c r="AK27" s="26"/>
-      <c r="AL27" s="27"/>
-      <c r="AM27" s="27"/>
-      <c r="AN27" s="27"/>
-      <c r="AO27" s="27"/>
-      <c r="AP27" s="27"/>
-      <c r="AQ27" s="26"/>
-      <c r="AR27" s="26"/>
-      <c r="AS27" s="26"/>
-      <c r="AT27" s="26"/>
-      <c r="AU27" s="26"/>
-      <c r="AV27" s="25"/>
-      <c r="AW27" s="25"/>
-      <c r="AX27" s="25"/>
-      <c r="AY27" s="25"/>
-      <c r="AZ27" s="25"/>
-      <c r="BA27" s="26"/>
-      <c r="BB27" s="26"/>
-      <c r="BC27" s="26"/>
-      <c r="BD27" s="26"/>
-      <c r="BE27" s="26"/>
-      <c r="BF27" s="27"/>
-      <c r="BG27" s="27"/>
-      <c r="BH27" s="27"/>
-      <c r="BI27" s="27"/>
-      <c r="BJ27" s="27"/>
-      <c r="BK27" s="26"/>
-      <c r="BL27" s="26"/>
-      <c r="BM27" s="26"/>
-      <c r="BN27" s="26"/>
-      <c r="BO27" s="28"/>
+      <c r="B27" s="85"/>
+      <c r="C27" s="100"/>
+      <c r="D27" s="101"/>
+      <c r="E27" s="101"/>
+      <c r="F27" s="101"/>
+      <c r="G27" s="101"/>
+      <c r="H27" s="31"/>
+      <c r="I27" s="32"/>
+      <c r="J27" s="33"/>
+      <c r="K27" s="33"/>
+      <c r="L27" s="72"/>
+      <c r="M27" s="72"/>
+      <c r="N27" s="72"/>
+      <c r="O27" s="72"/>
+      <c r="P27" s="72"/>
+      <c r="Q27" s="72"/>
+      <c r="R27" s="72"/>
+      <c r="S27" s="31"/>
+      <c r="T27" s="31"/>
+      <c r="U27" s="31"/>
+      <c r="V27" s="31"/>
+      <c r="W27" s="31"/>
+      <c r="X27" s="31"/>
+      <c r="Y27" s="31"/>
+      <c r="Z27" s="31"/>
+      <c r="AA27" s="31"/>
+      <c r="AB27" s="31"/>
+      <c r="AC27" s="31"/>
+      <c r="AD27" s="31"/>
+      <c r="AE27" s="31"/>
+      <c r="AF27" s="31"/>
+      <c r="AG27" s="31"/>
+      <c r="AH27" s="31"/>
+      <c r="AI27" s="31"/>
+      <c r="AJ27" s="31"/>
+      <c r="AK27" s="31"/>
+      <c r="AL27" s="31"/>
+      <c r="AM27" s="31"/>
+      <c r="AN27" s="31"/>
+      <c r="AO27" s="31"/>
+      <c r="AP27" s="31"/>
+      <c r="AQ27" s="31"/>
+      <c r="AR27" s="31"/>
+      <c r="AS27" s="31"/>
+      <c r="AT27" s="31"/>
+      <c r="AU27" s="31"/>
+      <c r="AV27" s="31"/>
+      <c r="AW27" s="31"/>
+      <c r="AX27" s="31"/>
+      <c r="AY27" s="31"/>
+      <c r="AZ27" s="31"/>
+      <c r="BA27" s="31"/>
+      <c r="BB27" s="31"/>
+      <c r="BC27" s="31"/>
+      <c r="BD27" s="31"/>
+      <c r="BE27" s="31"/>
+      <c r="BF27" s="31"/>
+      <c r="BG27" s="31"/>
+      <c r="BH27" s="31"/>
+      <c r="BI27" s="31"/>
+      <c r="BJ27" s="31"/>
+      <c r="BK27" s="31"/>
+      <c r="BL27" s="31"/>
+      <c r="BM27" s="31"/>
+      <c r="BN27" s="31"/>
+      <c r="BO27" s="31"/>
     </row>
     <row r="28" spans="1:67" s="84" customFormat="1" ht="14.35">
       <c r="B28" s="19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C28" s="34">
-        <v>43781</v>
+        <v>43780</v>
       </c>
       <c r="D28" s="34">
         <v>43800</v>
       </c>
       <c r="E28" s="21">
-        <f t="shared" ref="E28:E31" si="3">NETWORKDAYS(C28,D28)</f>
-        <v>14</v>
+        <f>NETWORKDAYS(C28,D28)</f>
+        <v>15</v>
       </c>
       <c r="F28" s="19" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="G28" s="35">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H28" s="23"/>
       <c r="I28" s="24"/>
@@ -7049,15 +7051,15 @@
       <c r="P28" s="26"/>
       <c r="Q28" s="26"/>
       <c r="R28" s="25"/>
-      <c r="S28" s="71"/>
+      <c r="S28" s="25"/>
       <c r="T28" s="25"/>
       <c r="U28" s="25"/>
-      <c r="V28" s="25"/>
-      <c r="W28" s="26"/>
-      <c r="X28" s="26"/>
-      <c r="Y28" s="26"/>
-      <c r="Z28" s="26"/>
-      <c r="AA28" s="26"/>
+      <c r="V28" s="27"/>
+      <c r="W28" s="73"/>
+      <c r="X28" s="73"/>
+      <c r="Y28" s="73"/>
+      <c r="Z28" s="73"/>
+      <c r="AA28" s="73"/>
       <c r="AB28" s="27"/>
       <c r="AC28" s="27"/>
       <c r="AD28" s="27"/>
@@ -7101,28 +7103,28 @@
     </row>
     <row r="29" spans="1:67" s="84" customFormat="1" ht="14.35">
       <c r="B29" s="19" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C29" s="34">
-        <v>43780</v>
+        <v>43781</v>
       </c>
       <c r="D29" s="34">
         <v>43800</v>
       </c>
       <c r="E29" s="21">
-        <f t="shared" si="3"/>
-        <v>15</v>
+        <f t="shared" ref="E29:E32" si="3">NETWORKDAYS(C29,D29)</f>
+        <v>14</v>
       </c>
       <c r="F29" s="19" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="G29" s="35">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="H29" s="23"/>
       <c r="I29" s="24"/>
       <c r="J29" s="25"/>
-      <c r="K29" s="75"/>
+      <c r="K29" s="25"/>
       <c r="L29" s="25"/>
       <c r="M29" s="26"/>
       <c r="N29" s="26"/>
@@ -7130,15 +7132,15 @@
       <c r="P29" s="26"/>
       <c r="Q29" s="26"/>
       <c r="R29" s="25"/>
-      <c r="S29" s="25"/>
+      <c r="S29" s="71"/>
       <c r="T29" s="25"/>
       <c r="U29" s="25"/>
-      <c r="V29" s="25"/>
-      <c r="W29" s="26"/>
-      <c r="X29" s="26"/>
-      <c r="Y29" s="26"/>
-      <c r="Z29" s="26"/>
-      <c r="AA29" s="26"/>
+      <c r="V29" s="27"/>
+      <c r="W29" s="73"/>
+      <c r="X29" s="73"/>
+      <c r="Y29" s="73"/>
+      <c r="Z29" s="73"/>
+      <c r="AA29" s="73"/>
       <c r="AB29" s="27"/>
       <c r="AC29" s="27"/>
       <c r="AD29" s="27"/>
@@ -7182,23 +7184,23 @@
     </row>
     <row r="30" spans="1:67" s="84" customFormat="1" ht="14.35">
       <c r="B30" s="19" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C30" s="34">
-        <v>43783</v>
+        <v>43780</v>
       </c>
       <c r="D30" s="34">
         <v>43800</v>
       </c>
       <c r="E30" s="21">
         <f t="shared" si="3"/>
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F30" s="19" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="G30" s="35">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H30" s="23"/>
       <c r="I30" s="24"/>
@@ -7214,12 +7216,12 @@
       <c r="S30" s="25"/>
       <c r="T30" s="25"/>
       <c r="U30" s="25"/>
-      <c r="V30" s="25"/>
-      <c r="W30" s="26"/>
-      <c r="X30" s="26"/>
-      <c r="Y30" s="26"/>
-      <c r="Z30" s="26"/>
-      <c r="AA30" s="26"/>
+      <c r="V30" s="27"/>
+      <c r="W30" s="73"/>
+      <c r="X30" s="73"/>
+      <c r="Y30" s="73"/>
+      <c r="Z30" s="73"/>
+      <c r="AA30" s="73"/>
       <c r="AB30" s="27"/>
       <c r="AC30" s="27"/>
       <c r="AD30" s="27"/>
@@ -7263,23 +7265,23 @@
     </row>
     <row r="31" spans="1:67" s="84" customFormat="1" ht="14.35">
       <c r="B31" s="19" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C31" s="34">
-        <v>43784</v>
+        <v>43783</v>
       </c>
       <c r="D31" s="34">
         <v>43800</v>
       </c>
       <c r="E31" s="21">
         <f t="shared" si="3"/>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F31" s="19" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="G31" s="35">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H31" s="23"/>
       <c r="I31" s="24"/>
@@ -7295,12 +7297,12 @@
       <c r="S31" s="25"/>
       <c r="T31" s="25"/>
       <c r="U31" s="25"/>
-      <c r="V31" s="25"/>
-      <c r="W31" s="26"/>
-      <c r="X31" s="26"/>
-      <c r="Y31" s="26"/>
-      <c r="Z31" s="26"/>
-      <c r="AA31" s="26"/>
+      <c r="V31" s="27"/>
+      <c r="W31" s="73"/>
+      <c r="X31" s="73"/>
+      <c r="Y31" s="73"/>
+      <c r="Z31" s="73"/>
+      <c r="AA31" s="73"/>
       <c r="AB31" s="27"/>
       <c r="AC31" s="27"/>
       <c r="AD31" s="27"/>
@@ -7342,55 +7344,211 @@
       <c r="BN31" s="26"/>
       <c r="BO31" s="28"/>
     </row>
-    <row r="32" spans="1:67" ht="12.7">
-      <c r="A32" s="46"/>
-    </row>
-    <row r="33" spans="1:1" ht="12.7">
-      <c r="A33" s="46"/>
-    </row>
-    <row r="34" spans="1:1" ht="12.7">
+    <row r="32" spans="1:67" s="84" customFormat="1" ht="14.35">
+      <c r="B32" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="C32" s="34">
+        <v>43784</v>
+      </c>
+      <c r="D32" s="34">
+        <v>43800</v>
+      </c>
+      <c r="E32" s="21">
+        <f t="shared" si="3"/>
+        <v>11</v>
+      </c>
+      <c r="F32" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="G32" s="35">
+        <v>1</v>
+      </c>
+      <c r="H32" s="23"/>
+      <c r="I32" s="24"/>
+      <c r="J32" s="25"/>
+      <c r="K32" s="75"/>
+      <c r="L32" s="25"/>
+      <c r="M32" s="26"/>
+      <c r="N32" s="26"/>
+      <c r="O32" s="26"/>
+      <c r="P32" s="26"/>
+      <c r="Q32" s="26"/>
+      <c r="R32" s="25"/>
+      <c r="S32" s="25"/>
+      <c r="T32" s="25"/>
+      <c r="U32" s="25"/>
+      <c r="V32" s="27"/>
+      <c r="W32" s="73"/>
+      <c r="X32" s="73"/>
+      <c r="Y32" s="73"/>
+      <c r="Z32" s="73"/>
+      <c r="AA32" s="73"/>
+      <c r="AB32" s="27"/>
+      <c r="AC32" s="27"/>
+      <c r="AD32" s="27"/>
+      <c r="AE32" s="27"/>
+      <c r="AF32" s="27"/>
+      <c r="AG32" s="26"/>
+      <c r="AH32" s="26"/>
+      <c r="AI32" s="26"/>
+      <c r="AJ32" s="26"/>
+      <c r="AK32" s="26"/>
+      <c r="AL32" s="27"/>
+      <c r="AM32" s="27"/>
+      <c r="AN32" s="27"/>
+      <c r="AO32" s="27"/>
+      <c r="AP32" s="27"/>
+      <c r="AQ32" s="26"/>
+      <c r="AR32" s="26"/>
+      <c r="AS32" s="26"/>
+      <c r="AT32" s="26"/>
+      <c r="AU32" s="26"/>
+      <c r="AV32" s="25"/>
+      <c r="AW32" s="25"/>
+      <c r="AX32" s="25"/>
+      <c r="AY32" s="25"/>
+      <c r="AZ32" s="25"/>
+      <c r="BA32" s="26"/>
+      <c r="BB32" s="26"/>
+      <c r="BC32" s="26"/>
+      <c r="BD32" s="26"/>
+      <c r="BE32" s="26"/>
+      <c r="BF32" s="27"/>
+      <c r="BG32" s="27"/>
+      <c r="BH32" s="27"/>
+      <c r="BI32" s="27"/>
+      <c r="BJ32" s="27"/>
+      <c r="BK32" s="26"/>
+      <c r="BL32" s="26"/>
+      <c r="BM32" s="26"/>
+      <c r="BN32" s="26"/>
+      <c r="BO32" s="28"/>
+    </row>
+    <row r="33" spans="1:67" s="87" customFormat="1" ht="14.35">
+      <c r="B33" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="C33" s="34">
+        <v>43784</v>
+      </c>
+      <c r="D33" s="34">
+        <v>43800</v>
+      </c>
+      <c r="E33" s="21">
+        <f t="shared" ref="E33" si="4">NETWORKDAYS(C33,D33)</f>
+        <v>11</v>
+      </c>
+      <c r="F33" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="G33" s="35">
+        <v>1</v>
+      </c>
+      <c r="H33" s="23"/>
+      <c r="I33" s="24"/>
+      <c r="J33" s="25"/>
+      <c r="K33" s="75"/>
+      <c r="L33" s="25"/>
+      <c r="M33" s="26"/>
+      <c r="N33" s="26"/>
+      <c r="O33" s="26"/>
+      <c r="P33" s="26"/>
+      <c r="Q33" s="26"/>
+      <c r="R33" s="25"/>
+      <c r="S33" s="25"/>
+      <c r="T33" s="25"/>
+      <c r="U33" s="25"/>
+      <c r="V33" s="27"/>
+      <c r="W33" s="73"/>
+      <c r="X33" s="73"/>
+      <c r="Y33" s="73"/>
+      <c r="Z33" s="73"/>
+      <c r="AA33" s="73"/>
+      <c r="AB33" s="27"/>
+      <c r="AC33" s="27"/>
+      <c r="AD33" s="27"/>
+      <c r="AE33" s="27"/>
+      <c r="AF33" s="27"/>
+      <c r="AG33" s="26"/>
+      <c r="AH33" s="26"/>
+      <c r="AI33" s="26"/>
+      <c r="AJ33" s="26"/>
+      <c r="AK33" s="26"/>
+      <c r="AL33" s="27"/>
+      <c r="AM33" s="27"/>
+      <c r="AN33" s="27"/>
+      <c r="AO33" s="27"/>
+      <c r="AP33" s="27"/>
+      <c r="AQ33" s="26"/>
+      <c r="AR33" s="26"/>
+      <c r="AS33" s="26"/>
+      <c r="AT33" s="26"/>
+      <c r="AU33" s="26"/>
+      <c r="AV33" s="25"/>
+      <c r="AW33" s="25"/>
+      <c r="AX33" s="25"/>
+      <c r="AY33" s="25"/>
+      <c r="AZ33" s="25"/>
+      <c r="BA33" s="26"/>
+      <c r="BB33" s="26"/>
+      <c r="BC33" s="26"/>
+      <c r="BD33" s="26"/>
+      <c r="BE33" s="26"/>
+      <c r="BF33" s="27"/>
+      <c r="BG33" s="27"/>
+      <c r="BH33" s="27"/>
+      <c r="BI33" s="27"/>
+      <c r="BJ33" s="27"/>
+      <c r="BK33" s="26"/>
+      <c r="BL33" s="26"/>
+      <c r="BM33" s="26"/>
+      <c r="BN33" s="26"/>
+      <c r="BO33" s="28"/>
+    </row>
+    <row r="34" spans="1:67" ht="12.7">
       <c r="A34" s="46"/>
     </row>
-    <row r="35" spans="1:1" ht="12.7">
+    <row r="35" spans="1:67" ht="12.7">
       <c r="A35" s="46"/>
     </row>
-    <row r="36" spans="1:1" ht="12.7">
+    <row r="36" spans="1:67" ht="12.7">
       <c r="A36" s="46"/>
     </row>
-    <row r="37" spans="1:1" ht="12.7">
+    <row r="37" spans="1:67" ht="12.7">
       <c r="A37" s="46"/>
     </row>
-    <row r="38" spans="1:1" ht="12.7">
+    <row r="38" spans="1:67" ht="12.7">
       <c r="A38" s="46"/>
     </row>
-    <row r="39" spans="1:1" ht="12.7">
+    <row r="39" spans="1:67" ht="12.7">
       <c r="A39" s="46"/>
     </row>
-    <row r="40" spans="1:1" ht="12.7">
+    <row r="40" spans="1:67" ht="12.7">
       <c r="A40" s="46"/>
     </row>
-    <row r="41" spans="1:1" ht="12.7">
+    <row r="41" spans="1:67" ht="12.7">
       <c r="A41" s="46"/>
     </row>
-    <row r="42" spans="1:1" ht="12.7">
+    <row r="42" spans="1:67" ht="12.7">
       <c r="A42" s="46"/>
     </row>
-    <row r="43" spans="1:1" ht="12.7">
+    <row r="43" spans="1:67" ht="12.7">
       <c r="A43" s="46"/>
     </row>
-    <row r="44" spans="1:1" ht="12.7">
+    <row r="44" spans="1:67" ht="12.7">
       <c r="A44" s="46"/>
     </row>
-    <row r="45" spans="1:1" ht="12.7">
+    <row r="45" spans="1:67" ht="12.7">
       <c r="A45" s="46"/>
     </row>
-    <row r="46" spans="1:1" ht="12.7">
+    <row r="46" spans="1:67" ht="12.7">
       <c r="A46" s="46"/>
     </row>
-    <row r="47" spans="1:1" ht="12.7">
+    <row r="47" spans="1:67" ht="12.7">
       <c r="A47" s="46"/>
     </row>
-    <row r="48" spans="1:1" ht="12.7">
+    <row r="48" spans="1:67" ht="12.7">
       <c r="A48" s="46"/>
     </row>
     <row r="49" spans="1:1" ht="12.7">
@@ -10149,69 +10307,69 @@
     </row>
     <row r="967" spans="1:67" ht="12.7">
       <c r="A967" s="46"/>
-      <c r="H967" s="4"/>
-      <c r="I967" s="4"/>
-      <c r="J967" s="4"/>
-      <c r="K967" s="4"/>
-      <c r="L967" s="4"/>
-      <c r="M967" s="4"/>
-      <c r="N967" s="4"/>
-      <c r="O967" s="4"/>
-      <c r="P967" s="4"/>
-      <c r="Q967" s="4"/>
-      <c r="R967" s="4"/>
-      <c r="S967" s="4"/>
-      <c r="T967" s="4"/>
-      <c r="U967" s="4"/>
-      <c r="V967" s="4"/>
-      <c r="W967" s="4"/>
-      <c r="X967" s="4"/>
-      <c r="Y967" s="4"/>
-      <c r="Z967" s="4"/>
-      <c r="AA967" s="4"/>
-      <c r="AB967" s="4"/>
-      <c r="AC967" s="4"/>
-      <c r="AD967" s="4"/>
-      <c r="AE967" s="4"/>
-      <c r="AF967" s="4"/>
-      <c r="AG967" s="4"/>
-      <c r="AH967" s="4"/>
-      <c r="AI967" s="4"/>
-      <c r="AJ967" s="4"/>
-      <c r="AK967" s="4"/>
-      <c r="AL967" s="4"/>
-      <c r="AM967" s="4"/>
-      <c r="AN967" s="4"/>
-      <c r="AO967" s="4"/>
-      <c r="AP967" s="4"/>
-      <c r="AQ967" s="4"/>
-      <c r="AR967" s="4"/>
-      <c r="AS967" s="4"/>
-      <c r="AT967" s="4"/>
-      <c r="AU967" s="4"/>
-      <c r="AV967" s="4"/>
-      <c r="AW967" s="4"/>
-      <c r="AX967" s="4"/>
-      <c r="AY967" s="4"/>
-      <c r="AZ967" s="4"/>
-      <c r="BA967" s="4"/>
-      <c r="BB967" s="4"/>
-      <c r="BC967" s="4"/>
-      <c r="BD967" s="4"/>
-      <c r="BE967" s="4"/>
-      <c r="BF967" s="4"/>
-      <c r="BG967" s="4"/>
-      <c r="BH967" s="4"/>
-      <c r="BI967" s="4"/>
-      <c r="BJ967" s="4"/>
-      <c r="BK967" s="4"/>
-      <c r="BL967" s="4"/>
-      <c r="BM967" s="4"/>
-      <c r="BN967" s="4"/>
-      <c r="BO967" s="4"/>
     </row>
     <row r="968" spans="1:67" ht="12.7">
       <c r="A968" s="46"/>
+      <c r="H968" s="4"/>
+      <c r="I968" s="4"/>
+      <c r="J968" s="4"/>
+      <c r="K968" s="4"/>
+      <c r="L968" s="4"/>
+      <c r="M968" s="4"/>
+      <c r="N968" s="4"/>
+      <c r="O968" s="4"/>
+      <c r="P968" s="4"/>
+      <c r="Q968" s="4"/>
+      <c r="R968" s="4"/>
+      <c r="S968" s="4"/>
+      <c r="T968" s="4"/>
+      <c r="U968" s="4"/>
+      <c r="V968" s="4"/>
+      <c r="W968" s="4"/>
+      <c r="X968" s="4"/>
+      <c r="Y968" s="4"/>
+      <c r="Z968" s="4"/>
+      <c r="AA968" s="4"/>
+      <c r="AB968" s="4"/>
+      <c r="AC968" s="4"/>
+      <c r="AD968" s="4"/>
+      <c r="AE968" s="4"/>
+      <c r="AF968" s="4"/>
+      <c r="AG968" s="4"/>
+      <c r="AH968" s="4"/>
+      <c r="AI968" s="4"/>
+      <c r="AJ968" s="4"/>
+      <c r="AK968" s="4"/>
+      <c r="AL968" s="4"/>
+      <c r="AM968" s="4"/>
+      <c r="AN968" s="4"/>
+      <c r="AO968" s="4"/>
+      <c r="AP968" s="4"/>
+      <c r="AQ968" s="4"/>
+      <c r="AR968" s="4"/>
+      <c r="AS968" s="4"/>
+      <c r="AT968" s="4"/>
+      <c r="AU968" s="4"/>
+      <c r="AV968" s="4"/>
+      <c r="AW968" s="4"/>
+      <c r="AX968" s="4"/>
+      <c r="AY968" s="4"/>
+      <c r="AZ968" s="4"/>
+      <c r="BA968" s="4"/>
+      <c r="BB968" s="4"/>
+      <c r="BC968" s="4"/>
+      <c r="BD968" s="4"/>
+      <c r="BE968" s="4"/>
+      <c r="BF968" s="4"/>
+      <c r="BG968" s="4"/>
+      <c r="BH968" s="4"/>
+      <c r="BI968" s="4"/>
+      <c r="BJ968" s="4"/>
+      <c r="BK968" s="4"/>
+      <c r="BL968" s="4"/>
+      <c r="BM968" s="4"/>
+      <c r="BN968" s="4"/>
+      <c r="BO968" s="4"/>
     </row>
     <row r="969" spans="1:67" ht="12.7">
       <c r="A969" s="46"/>
@@ -10277,17 +10435,20 @@
       <c r="A989" s="46"/>
     </row>
     <row r="990" spans="1:7" ht="12.7">
-      <c r="A990" s="66"/>
-      <c r="B990" s="4"/>
-      <c r="C990" s="4"/>
-      <c r="D990" s="4"/>
-      <c r="E990" s="4"/>
-      <c r="F990" s="4"/>
-      <c r="G990" s="4"/>
+      <c r="A990" s="46"/>
+    </row>
+    <row r="991" spans="1:7" ht="12.7">
+      <c r="A991" s="66"/>
+      <c r="B991" s="4"/>
+      <c r="C991" s="4"/>
+      <c r="D991" s="4"/>
+      <c r="E991" s="4"/>
+      <c r="F991" s="4"/>
+      <c r="G991" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="C26:G26"/>
+    <mergeCell ref="C27:G27"/>
     <mergeCell ref="C21:G21"/>
     <mergeCell ref="C15:G15"/>
     <mergeCell ref="C8:G8"/>
@@ -10312,8 +10473,8 @@
     <mergeCell ref="AB6:AF6"/>
     <mergeCell ref="R6:V6"/>
   </mergeCells>
-  <conditionalFormatting sqref="G22:G25 G16:G20 G9:G14">
-    <cfRule type="colorScale" priority="4">
+  <conditionalFormatting sqref="G16:G20 G9:G14 G22:G26">
+    <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="100"/>
@@ -10322,8 +10483,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G27:G31">
-    <cfRule type="colorScale" priority="2">
+  <conditionalFormatting sqref="G28:G33">
+    <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="100"/>

</xml_diff>